<commit_message>
Optimized the code and fixed the delete button and recent entry section.
</commit_message>
<xml_diff>
--- a/static/db.xlsx
+++ b/static/db.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>KLZ6 E 200</t>
+          <t>KL51J6070</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-10-31</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>09:16:47</t>
+          <t>14:05:55</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,249 +481,58 @@
           <t>IN</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1730346407911</t>
-        </is>
+      <c r="E2" t="n">
+        <v>1731918955392</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>KLZ6 E 200</t>
+          <t>MH01s1513</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-10-31</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>09:16:59</t>
+          <t>14:09:10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1730346419340</t>
-        </is>
+          <t>IN</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1731919150890</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>~6J02e30563</t>
+          <t>Mh01s1513</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2024-11-06</t>
+          <t>2024-11-18</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>15:30:16</t>
+          <t>14:09:34</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1730887216669</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RJo7 € 3258</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>15:30:30</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1730887230523</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>6JO3ER0563</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>15:30:55</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
           <t>OUT</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1730887255283</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>15:31:13</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1730887273891</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Thoreo</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>15:31:20</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1730887280323</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>23BH0121E</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>15:31:26</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1730887286068</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>56ZEDL</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>15:55:05</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>IN</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1730888705263</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>S6ZEDL</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2024-11-06</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>15:55:32</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>OUT</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1730888732732</t>
-        </is>
+      <c r="E4" t="n">
+        <v>1731919174136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>